<commit_message>
Updates WBS & Breakdown Chart
</commit_message>
<xml_diff>
--- a/Conception/Gestion de Projet/Burndown Chart.xlsx
+++ b/Conception/Gestion de Projet/Burndown Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Desktop\Exia\A4\UE 2\Projet Embarqué\Git Projet Embarqué\Conception\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Desktop\Exia\A4\UE 2\Projet Embarqué\Git Projet Embarqué\Conception\Gestion de Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -165,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,14 +178,6 @@
       <u/>
       <sz val="11"/>
       <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,28 +224,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <i val="0"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1628,7 +1626,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="R1:U36" totalsRowShown="0">
   <autoFilter ref="R1:U36"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="ID"/>
+    <tableColumn id="1" name="ID" dataDxfId="0"/>
     <tableColumn id="2" name="Tasks"/>
     <tableColumn id="3" name="Days required"/>
     <tableColumn id="4" name="Day done"/>
@@ -1936,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,18 +1949,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="R1" t="s">
@@ -1979,21 +1977,22 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="S2" s="6" t="s">
+      <c r="F2" s="8"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2009,16 +2008,16 @@
         <v>28</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="R3" s="7">
-        <v>1</v>
-      </c>
-      <c r="S3" s="9" t="s">
+      <c r="R3" s="6">
+        <v>1</v>
+      </c>
+      <c r="S3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="9">
-        <v>1</v>
-      </c>
-      <c r="U3" s="5">
+      <c r="T3" s="6">
+        <v>1</v>
+      </c>
+      <c r="U3" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2044,16 +2043,16 @@
         <f>E3-E4</f>
         <v>3</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
         <v>2</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="S4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="9">
-        <v>1</v>
-      </c>
-      <c r="U4" s="5">
+      <c r="T4" s="6">
+        <v>1</v>
+      </c>
+      <c r="U4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2072,23 +2071,23 @@
         <v>20</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E14" si="0">E4-C5</f>
+        <f t="shared" ref="E5:E8" si="0">E4-C5</f>
         <v>21</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5:F8" si="1">E4-E5</f>
         <v>4</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="3">
         <v>3</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="T5" s="5">
-        <v>1</v>
-      </c>
-      <c r="U5" s="5">
+      <c r="T5" s="3">
+        <v>1</v>
+      </c>
+      <c r="U5" s="3">
         <v>2</v>
       </c>
     </row>
@@ -2114,16 +2113,16 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="3">
         <v>4</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="5">
-        <v>1</v>
-      </c>
-      <c r="U6" s="5">
+      <c r="T6" s="3">
+        <v>1</v>
+      </c>
+      <c r="U6" s="3">
         <v>10</v>
       </c>
     </row>
@@ -2149,16 +2148,16 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="3">
         <v>5</v>
       </c>
-      <c r="S7" s="5" t="s">
+      <c r="S7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="T7" s="5">
-        <v>1</v>
-      </c>
-      <c r="U7" s="5">
+      <c r="T7" s="3">
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
         <v>10</v>
       </c>
     </row>
@@ -2184,16 +2183,16 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="3">
         <v>6</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="T8" s="5">
-        <v>1</v>
-      </c>
-      <c r="U8" s="5">
+      <c r="T8" s="3">
+        <v>1</v>
+      </c>
+      <c r="U8" s="3">
         <v>8</v>
       </c>
     </row>
@@ -2211,11 +2210,12 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="S9" s="6" t="s">
+      <c r="R9" s="3"/>
+      <c r="S9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -2231,16 +2231,16 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="R10" s="7">
+      <c r="R10" s="6">
         <v>7</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="S10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="T10" s="9">
-        <v>1</v>
-      </c>
-      <c r="U10" s="5">
+      <c r="T10" s="6">
+        <v>1</v>
+      </c>
+      <c r="U10" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2258,16 +2258,16 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="R11">
+      <c r="R11" s="3">
         <v>8</v>
       </c>
-      <c r="S11" s="5" t="s">
+      <c r="S11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T11" s="5">
+      <c r="T11" s="3">
         <v>3</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U11" s="3">
         <v>3</v>
       </c>
     </row>
@@ -2285,16 +2285,16 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="R12">
+      <c r="R12" s="3">
         <v>9</v>
       </c>
-      <c r="S12" s="5" t="s">
+      <c r="S12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T12" s="5">
+      <c r="T12" s="3">
         <v>3</v>
       </c>
-      <c r="U12" s="5">
+      <c r="U12" s="3">
         <v>3</v>
       </c>
     </row>
@@ -2312,16 +2312,16 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="R13">
+      <c r="R13" s="3">
         <v>10</v>
       </c>
-      <c r="S13" s="5" t="s">
+      <c r="S13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T13" s="5">
+      <c r="T13" s="3">
         <v>4</v>
       </c>
-      <c r="U13" s="5">
+      <c r="U13" s="3">
         <v>7</v>
       </c>
     </row>
@@ -2339,308 +2339,312 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="R14">
+      <c r="R14" s="3">
         <v>11</v>
       </c>
-      <c r="S14" s="5" t="s">
+      <c r="S14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T14" s="5">
+      <c r="T14" s="3">
         <v>4</v>
       </c>
-      <c r="U14" s="5">
+      <c r="U14" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="S15" s="6" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="R16" s="7">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="R16" s="6">
         <v>12</v>
       </c>
-      <c r="S16" s="9" t="s">
+      <c r="S16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="T16" s="9">
-        <v>1</v>
-      </c>
-      <c r="U16" s="5">
+      <c r="T16" s="6">
+        <v>1</v>
+      </c>
+      <c r="U16" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R17">
+      <c r="R17" s="3">
         <v>13</v>
       </c>
-      <c r="S17" s="5" t="s">
+      <c r="S17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="T17" s="5">
-        <v>1</v>
-      </c>
-      <c r="U17" s="5">
+      <c r="T17" s="3">
+        <v>1</v>
+      </c>
+      <c r="U17" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R18">
+      <c r="R18" s="3">
         <v>14</v>
       </c>
-      <c r="S18" s="5" t="s">
+      <c r="S18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="5">
-        <v>1</v>
-      </c>
-      <c r="U18" s="5">
+      <c r="T18" s="3">
+        <v>1</v>
+      </c>
+      <c r="U18" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R19">
+      <c r="R19" s="3">
         <v>15</v>
       </c>
-      <c r="S19" s="5" t="s">
+      <c r="S19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T19" s="5">
-        <v>1</v>
-      </c>
-      <c r="U19" s="5">
+      <c r="T19" s="3">
+        <v>1</v>
+      </c>
+      <c r="U19" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R20">
+      <c r="R20" s="3">
         <v>16</v>
       </c>
-      <c r="S20" s="5" t="s">
+      <c r="S20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="T20" s="5">
-        <v>1</v>
-      </c>
-      <c r="U20" s="5">
+      <c r="T20" s="3">
+        <v>1</v>
+      </c>
+      <c r="U20" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R21">
+      <c r="R21" s="3">
         <v>17</v>
       </c>
-      <c r="S21" s="5" t="s">
+      <c r="S21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T21" s="5">
+      <c r="T21" s="3">
         <v>2</v>
       </c>
-      <c r="U21" s="5">
+      <c r="U21" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="S22" s="6" t="s">
+      <c r="R22" s="3"/>
+      <c r="S22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
     </row>
     <row r="23" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R23">
+      <c r="R23" s="3">
         <v>18</v>
       </c>
-      <c r="S23" s="5" t="s">
+      <c r="S23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T23" s="5">
-        <v>1</v>
-      </c>
-      <c r="U23" s="5">
+      <c r="T23" s="3">
+        <v>1</v>
+      </c>
+      <c r="U23" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R24">
+      <c r="R24" s="3">
         <v>19</v>
       </c>
-      <c r="S24" s="5" t="s">
+      <c r="S24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="T24" s="5">
-        <v>1</v>
-      </c>
-      <c r="U24" s="5">
+      <c r="T24" s="3">
+        <v>1</v>
+      </c>
+      <c r="U24" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R25">
+      <c r="R25" s="3">
         <v>20</v>
       </c>
-      <c r="S25" s="5" t="s">
+      <c r="S25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="T25" s="5">
+      <c r="T25" s="3">
         <v>2</v>
       </c>
-      <c r="U25" s="5">
+      <c r="U25" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R26">
+      <c r="R26" s="3">
         <v>21</v>
       </c>
-      <c r="S26" s="5" t="s">
+      <c r="S26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="3">
         <v>3</v>
       </c>
-      <c r="U26" s="5">
+      <c r="U26" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R27">
+      <c r="R27" s="3">
         <v>22</v>
       </c>
-      <c r="S27" s="5" t="s">
+      <c r="S27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T27" s="5">
+      <c r="T27" s="3">
         <v>2</v>
       </c>
-      <c r="U27" s="5">
+      <c r="U27" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="S28" s="6" t="s">
+      <c r="R28" s="3"/>
+      <c r="S28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
     </row>
     <row r="29" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R29">
+      <c r="R29" s="3">
         <v>23</v>
       </c>
-      <c r="S29" s="5" t="s">
+      <c r="S29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="T29" s="5">
-        <v>1</v>
-      </c>
-      <c r="U29" s="5">
+      <c r="T29" s="3">
+        <v>1</v>
+      </c>
+      <c r="U29" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R30">
+      <c r="R30" s="3">
         <v>24</v>
       </c>
-      <c r="S30" s="5" t="s">
+      <c r="S30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="T30" s="5">
+      <c r="T30" s="3">
         <v>2</v>
       </c>
-      <c r="U30" s="5">
+      <c r="U30" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R31">
+      <c r="R31" s="3">
         <v>25</v>
       </c>
-      <c r="S31" s="5" t="s">
+      <c r="S31" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="T31" s="5">
+      <c r="T31" s="3">
         <v>2</v>
       </c>
-      <c r="U31" s="5">
+      <c r="U31" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="S32" s="6" t="s">
+      <c r="R32" s="3"/>
+      <c r="S32" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
     </row>
     <row r="33" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R33">
+      <c r="R33" s="3">
         <v>26</v>
       </c>
-      <c r="S33" s="5" t="s">
+      <c r="S33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="T33" s="5">
-        <v>1</v>
-      </c>
-      <c r="U33" s="5">
+      <c r="T33" s="3">
+        <v>1</v>
+      </c>
+      <c r="U33" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R34">
+      <c r="R34" s="3">
         <v>27</v>
       </c>
-      <c r="S34" s="5" t="s">
+      <c r="S34" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T34" s="5">
+      <c r="T34" s="3">
         <v>2</v>
       </c>
-      <c r="U34" s="5">
+      <c r="U34" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R35">
+      <c r="R35" s="3">
         <v>28</v>
       </c>
-      <c r="S35" s="5" t="s">
+      <c r="S35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T35" s="5">
-        <v>1</v>
-      </c>
-      <c r="U35" s="5">
+      <c r="T35" s="3">
+        <v>1</v>
+      </c>
+      <c r="U35" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R36">
+      <c r="R36" s="3">
         <v>29</v>
       </c>
-      <c r="S36" s="5" t="s">
+      <c r="S36" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="T36" s="5">
-        <v>1</v>
-      </c>
-      <c r="U36" s="5">
+      <c r="T36" s="3">
+        <v>1</v>
+      </c>
+      <c r="U36" s="3">
         <v>11</v>
       </c>
     </row>

</xml_diff>